<commit_message>
Correzione test case 150
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111DEDALUS0000/DEDALUS SPA/ARGOS/4.25.25706/report-checklist.xlsx
+++ b/GATEWAY/A1#111DEDALUS0000/DEDALUS SPA/ARGOS/4.25.25706/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Argos\argos\ASF Progetti\RSA-FSE\accreditamento\A1#111DEDALUS0000\DEDALUS SPA\ARGOS\4.25.25706\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3983B0F4-F6E6-4F88-A573-3C5866C20E12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E48D3F82-7DD5-4E1F-A5A8-89231B4AEA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29460" yWindow="60" windowWidth="22800" windowHeight="15240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -2044,19 +2044,19 @@
     <t>2024-11-13T17:20:16Z</t>
   </si>
   <si>
-    <t>2024-11-13T17:22:10Z</t>
-  </si>
-  <si>
     <t>cda45380af53ecc0</t>
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.90.4.4.cc082a3f46b908e61b33414542b81032fd9569b6733f2ce6cb901ef482924f66.8a0a9aad15^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>1d308d143c57a9af</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.90.4.4.cc082a3f46b908e61b33414542b81032fd9569b6733f2ce6cb901ef482924f66.4e9fc9affe^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2024-20-13T17:242:20Z</t>
+  </si>
+  <si>
+    <t>a3ce1aa798d66e89</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.90.4.4.cc082a3f46b908e61b33414542b81032fd9569b6733f2ce6cb901ef482924f66.b6d7a38837^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -4444,7 +4444,7 @@
   <dimension ref="A1:W809"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="78" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B151" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="F151" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
       <selection pane="bottomRight" activeCell="I153" sqref="I153"/>
@@ -10200,10 +10200,10 @@
         <v>532</v>
       </c>
       <c r="H152" s="33" t="s">
+        <v>533</v>
+      </c>
+      <c r="I152" s="33" t="s">
         <v>534</v>
-      </c>
-      <c r="I152" s="33" t="s">
-        <v>535</v>
       </c>
       <c r="J152" s="34" t="s">
         <v>87</v>
@@ -10243,10 +10243,10 @@
         <v>471</v>
       </c>
       <c r="F153" s="32">
-        <v>45609</v>
+        <v>45616</v>
       </c>
       <c r="G153" s="33" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="H153" s="33" t="s">
         <v>536</v>
@@ -19910,27 +19910,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -20188,32 +20167,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C8A108-5C92-4947-B020-8B796E060B59}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20230,4 +20205,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>